<commit_message>
020125 EOD added promotion order file
</commit_message>
<xml_diff>
--- a/Daily Activity/2024/DEC/31-12-24/CENTRA STATUS/QA_CENTRA_LQAT CheckList.xlsx
+++ b/Daily Activity/2024/DEC/31-12-24/CENTRA STATUS/QA_CENTRA_LQAT CheckList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="MasterData_CheckList" sheetId="1" state="visible" r:id="rId2"/>
@@ -2526,11 +2526,11 @@
   </sheetPr>
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.78"/>
@@ -4374,10 +4374,10 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.8"/>
@@ -5053,10 +5053,10 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.94"/>
@@ -5439,10 +5439,10 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.97"/>
@@ -6045,10 +6045,10 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.93"/>
@@ -6731,10 +6731,10 @@
   <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.8"/>
@@ -8015,11 +8015,11 @@
   </sheetPr>
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.3"/>
@@ -9100,10 +9100,10 @@
   <dimension ref="A1:K70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.02"/>
@@ -10756,10 +10756,10 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.8"/>
@@ -11884,10 +11884,10 @@
   <dimension ref="A1:J297"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.62"/>

</xml_diff>